<commit_message>
changes : add field 'iType' on masterdata barang
</commit_message>
<xml_diff>
--- a/public/template/FormatBarang.xlsx
+++ b/public/template/FormatBarang.xlsx
@@ -27,12 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Kode</t>
   </si>
   <si>
     <t>Nama</t>
+  </si>
+  <si>
+    <t>Tipe</t>
   </si>
   <si>
     <t>UoM</t>
@@ -939,6 +942,130 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Text Box 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4848225" y="209550"/>
+          <a:ext cx="3669030" cy="1190625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Kolom</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>	</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Keterangan</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>		</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Contoh</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Kode	Kode dari barang	K0001</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Nama	Nama dari Barang	Kursi Kayu</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Tipe	Jenis dari barang	Prasarana</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>UoM	Satuan dari barang	PCS</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1141,15 +1268,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C3"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="9" max="9" width="17.2857142857143" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:3">
+    <row r="1" customHeight="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1159,9 +1289,13 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>